<commit_message>
Hierarchy by children is working
</commit_message>
<xml_diff>
--- a/src/DirectUsage/files/Functions.xlsx
+++ b/src/DirectUsage/files/Functions.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="46080" windowHeight="22044"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10344" windowHeight="5436" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Per Parent" sheetId="1" r:id="rId1"/>
+    <sheet name="Per Child" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>Id</t>
   </si>
@@ -63,6 +64,12 @@
   </si>
   <si>
     <t>Radio</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>2,6,7,8,10</t>
   </si>
 </sst>
 </file>
@@ -416,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,4 +550,125 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel has Id, some refactoring
</commit_message>
<xml_diff>
--- a/src/DirectUsage/files/Functions.xlsx
+++ b/src/DirectUsage/files/Functions.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10344" windowHeight="5436" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10344" windowHeight="5436" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Per Parent" sheetId="1" r:id="rId1"/>
     <sheet name="Per Child" sheetId="2" r:id="rId2"/>
+    <sheet name="Länder" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
   <si>
     <t>Id</t>
   </si>
@@ -70,6 +71,180 @@
   </si>
   <si>
     <t>2,6,7,8,10</t>
+  </si>
+  <si>
+    <t>Deutschland</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Grüne und CDU</t>
+  </si>
+  <si>
+    <t>CSU</t>
+  </si>
+  <si>
+    <t>SPD und CDU</t>
+  </si>
+  <si>
+    <t>SPD und Linke</t>
+  </si>
+  <si>
+    <t>SPD und Grüne</t>
+  </si>
+  <si>
+    <t>SPD und Grüne (ehem. GAL)</t>
+  </si>
+  <si>
+    <t>CDU und Grüne</t>
+  </si>
+  <si>
+    <t>SPD, FDP und Grüne</t>
+  </si>
+  <si>
+    <t>CDU und SPD</t>
+  </si>
+  <si>
+    <t>CDU, SPD und Bündnis 90/Die Grünen</t>
+  </si>
+  <si>
+    <t>SPD, Grüne und SSW</t>
+  </si>
+  <si>
+    <t>Die Linke, SPD und Grüne</t>
+  </si>
+  <si>
+    <t>Regierung</t>
+  </si>
+  <si>
+    <t>Frankreich</t>
+  </si>
+  <si>
+    <t>Aquitaine (Aquitanien)</t>
+  </si>
+  <si>
+    <t>Auvergne</t>
+  </si>
+  <si>
+    <t>Basse-Normandie</t>
+  </si>
+  <si>
+    <t>Bretagne</t>
+  </si>
+  <si>
+    <t>Bourgogne (Burgund)</t>
+  </si>
+  <si>
+    <t>Centre-Val de Loire</t>
+  </si>
+  <si>
+    <t>Champagne-Ardenne</t>
+  </si>
+  <si>
+    <t>Alsace (Elsass)</t>
+  </si>
+  <si>
+    <t>Franche-Comté</t>
+  </si>
+  <si>
+    <t>Guyane (Französisch-Guayana)</t>
+  </si>
+  <si>
+    <t>Guadeloupe</t>
+  </si>
+  <si>
+    <t>Haute-Normandie</t>
+  </si>
+  <si>
+    <t>Île-de-France</t>
+  </si>
+  <si>
+    <t>Corse (Korsika)</t>
+  </si>
+  <si>
+    <t>Languedoc-Roussillon</t>
+  </si>
+  <si>
+    <t>Limousin</t>
+  </si>
+  <si>
+    <t>Lorraine (Lothringen)</t>
+  </si>
+  <si>
+    <t>Martinique</t>
+  </si>
+  <si>
+    <t>Mayotte</t>
+  </si>
+  <si>
+    <t>Midi-Pyrénées</t>
+  </si>
+  <si>
+    <t>Nord-Pas-de-Calais</t>
+  </si>
+  <si>
+    <t>Pays de la Loire</t>
+  </si>
+  <si>
+    <t>Picardie</t>
+  </si>
+  <si>
+    <t>Poitou-Charentes</t>
+  </si>
+  <si>
+    <t>Provence-Alpes-Côte d’Azur</t>
+  </si>
+  <si>
+    <t>Réunion</t>
+  </si>
+  <si>
+    <t>Rhône-Alpes</t>
   </si>
 </sst>
 </file>
@@ -556,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,4 +846,577 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>